<commit_message>
Minor updates to mapping spreadhsheet.
</commit_message>
<xml_diff>
--- a/shared/ojb-resources-common/src/main/resources/service-specifications/Incident_Reporting_Service/artifacts/service_model/information_model/Incident_Report_IEPD/documentation/impl-artifacts/vermont/Incident_Citation_Mapping.xlsx
+++ b/shared/ojb-resources-common/src/main/resources/service-specifications/Incident_Reporting_Service/artifacts/service_model/information_model/Incident_Report_IEPD/documentation/impl-artifacts/vermont/Incident_Citation_Mapping.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26519"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="4040" yWindow="1100" windowWidth="31480" windowHeight="17940"/>
+    <workbookView xWindow="-28800" yWindow="0" windowWidth="28800" windowHeight="18000"/>
   </bookViews>
   <sheets>
     <sheet name="Citation" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="285">
   <si>
     <t>Description</t>
   </si>
@@ -862,9 +862,6 @@
     <t xml:space="preserve"> /ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:StructuredPayload/inc-ext:IncidentReport/inc-ext:DriverLicense[lexslib:SameAsDigestReference/@lexslib:ref= /ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityPerson/lexsdigest:Person[@s:id = ../j:IncidentSubject/nc:RoleOfPersonReference/@s:ref]/j:PersonAugmentation/nc:DriverLicense/@s:id]/inc-ext:DriverLicenseCDLIndicator</t>
   </si>
   <si>
-    <t>TBD</t>
-  </si>
-  <si>
     <t>Civil Relief Act Juvenile Indicator</t>
   </si>
   <si>
@@ -887,6 +884,12 @@
   </si>
   <si>
     <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:StructuredPayload/inc-ext:IncidentReport/inc-ext:DrivingIncident[lexslib:SameAsDigestReference/@lexslib:ref=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityActivity/nc:Activity[nc:ActivityCategoryText='Incident']/@s:id]/inc-ext:CivilReliefActJuvenileIndicator</t>
+  </si>
+  <si>
+    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:StructuredPayload/inc-ext:IncidentReport/inc-ext:Charge/inc-ext:RelatedCriminalChargeIndicator</t>
+  </si>
+  <si>
+    <t>/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:EntityLocation/nc:Location[@s:id=/ir-doc:IncidentReport/lexspd:doPublish/lexs:PublishMessageContainer/lexs:PublishMessage/lexs:DataItemPackage/lexs:Digest/lexsdigest:Associations/lexsdigest:PersonBirthLocationAssociation/nc:LocationReference/@s:ref]/nc:LocationAddress/nc:StructuredAddress/nc:LocationCityName</t>
   </si>
 </sst>
 </file>
@@ -2517,9 +2520,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F87"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E63" sqref="E63"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -2958,7 +2961,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="28" spans="1:6" s="3" customFormat="1">
+    <row r="28" spans="1:6" s="3" customFormat="1" ht="84">
       <c r="A28" s="3" t="s">
         <v>158</v>
       </c>
@@ -2971,8 +2974,8 @@
       <c r="D28" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="E28" s="6" t="s">
-        <v>275</v>
+      <c r="E28" s="12" t="s">
+        <v>284</v>
       </c>
     </row>
     <row r="29" spans="1:6" s="3" customFormat="1" ht="70">
@@ -3468,7 +3471,7 @@
     </row>
     <row r="60" spans="1:6" ht="70">
       <c r="A60" s="7" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B60" s="2" t="s">
         <v>92</v>
@@ -3480,12 +3483,12 @@
         <v>1</v>
       </c>
       <c r="E60" s="12" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="61" spans="1:6" ht="70">
       <c r="A61" s="7" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B61" s="2" t="s">
         <v>93</v>
@@ -3497,12 +3500,12 @@
         <v>1</v>
       </c>
       <c r="E61" s="12" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="62" spans="1:6" ht="70">
       <c r="A62" s="7" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B62" s="2" t="s">
         <v>94</v>
@@ -3514,12 +3517,12 @@
         <v>1</v>
       </c>
       <c r="E62" s="11" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="63" spans="1:6" ht="70">
       <c r="A63" s="7" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B63" s="2" t="s">
         <v>186</v>
@@ -3528,7 +3531,7 @@
         <v>88</v>
       </c>
       <c r="E63" s="11" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="64" spans="1:6">
@@ -3609,7 +3612,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="69" spans="1:6" s="3" customFormat="1" ht="70">
+    <row r="69" spans="1:6" s="3" customFormat="1" ht="42">
       <c r="A69" s="6" t="s">
         <v>163</v>
       </c>
@@ -3623,7 +3626,7 @@
         <v>0</v>
       </c>
       <c r="E69" s="12" t="s">
-        <v>237</v>
+        <v>283</v>
       </c>
       <c r="F69" s="6"/>
     </row>

</xml_diff>